<commit_message>
Edited classes and ClassDiagramm
</commit_message>
<xml_diff>
--- a/Документация/Диаграмма Ганта.xlsx
+++ b/Документация/Диаграмма Ганта.xlsx
@@ -1,15 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="9303"/>
-  <workbookPr/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <workbookPr defaultThemeVersion="153222"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Mega\Warehouse_Automation\Документация\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7155"/>
   </bookViews>
   <sheets>
     <sheet name="Лист1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="145621"/>
+  <calcPr calcId="162913"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -102,9 +107,6 @@
     <t>Мельникова Ирина</t>
   </si>
   <si>
-    <t>Китцуль Даниил</t>
-  </si>
-  <si>
     <t>Распределение этапов анализа</t>
   </si>
   <si>
@@ -113,11 +115,14 @@
   <si>
     <t>Распределение этапов разработки докумнтации</t>
   </si>
+  <si>
+    <t>Кицуль Даниил</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="dd/mm/yy;@"/>
   </numFmts>
@@ -459,6 +464,15 @@
     <xf numFmtId="0" fontId="8" fillId="0" borderId="7" xfId="3" applyFont="1" applyBorder="1"/>
     <xf numFmtId="164" fontId="8" fillId="0" borderId="7" xfId="3" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="164" fontId="8" fillId="0" borderId="4" xfId="3" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="5" fillId="3" borderId="0" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -473,15 +487,6 @@
     </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="4">
@@ -504,7 +509,7 @@
 </file>
 
 <file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
   <c:lang val="ru-RU"/>
   <c:roundedCorners val="0"/>
@@ -647,6 +652,11 @@
               </c:numCache>
             </c:numRef>
           </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-988E-4A34-BC45-00A198917708}"/>
+            </c:ext>
+          </c:extLst>
         </c:ser>
         <c:ser>
           <c:idx val="1"/>
@@ -690,6 +700,11 @@
               </a:ln>
               <a:effectLst/>
             </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000002-988E-4A34-BC45-00A198917708}"/>
+              </c:ext>
+            </c:extLst>
           </c:dPt>
           <c:dPt>
             <c:idx val="1"/>
@@ -707,6 +722,11 @@
               </a:ln>
               <a:effectLst/>
             </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000004-988E-4A34-BC45-00A198917708}"/>
+              </c:ext>
+            </c:extLst>
           </c:dPt>
           <c:dPt>
             <c:idx val="2"/>
@@ -724,6 +744,11 @@
               </a:ln>
               <a:effectLst/>
             </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000006-988E-4A34-BC45-00A198917708}"/>
+              </c:ext>
+            </c:extLst>
           </c:dPt>
           <c:dPt>
             <c:idx val="3"/>
@@ -738,6 +763,11 @@
               </a:ln>
               <a:effectLst/>
             </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000008-988E-4A34-BC45-00A198917708}"/>
+              </c:ext>
+            </c:extLst>
           </c:dPt>
           <c:dPt>
             <c:idx val="4"/>
@@ -752,6 +782,11 @@
               </a:ln>
               <a:effectLst/>
             </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{0000000A-988E-4A34-BC45-00A198917708}"/>
+              </c:ext>
+            </c:extLst>
           </c:dPt>
           <c:dPt>
             <c:idx val="5"/>
@@ -769,6 +804,11 @@
               </a:ln>
               <a:effectLst/>
             </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{0000000C-988E-4A34-BC45-00A198917708}"/>
+              </c:ext>
+            </c:extLst>
           </c:dPt>
           <c:dPt>
             <c:idx val="6"/>
@@ -786,6 +826,11 @@
               </a:ln>
               <a:effectLst/>
             </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{0000000E-988E-4A34-BC45-00A198917708}"/>
+              </c:ext>
+            </c:extLst>
           </c:dPt>
           <c:dPt>
             <c:idx val="7"/>
@@ -800,6 +845,11 @@
               </a:ln>
               <a:effectLst/>
             </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000010-988E-4A34-BC45-00A198917708}"/>
+              </c:ext>
+            </c:extLst>
           </c:dPt>
           <c:dPt>
             <c:idx val="8"/>
@@ -817,6 +867,11 @@
               </a:ln>
               <a:effectLst/>
             </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000012-988E-4A34-BC45-00A198917708}"/>
+              </c:ext>
+            </c:extLst>
           </c:dPt>
           <c:dPt>
             <c:idx val="9"/>
@@ -831,6 +886,11 @@
               </a:ln>
               <a:effectLst/>
             </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000014-988E-4A34-BC45-00A198917708}"/>
+              </c:ext>
+            </c:extLst>
           </c:dPt>
           <c:dPt>
             <c:idx val="10"/>
@@ -845,6 +905,11 @@
               </a:ln>
               <a:effectLst/>
             </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000016-988E-4A34-BC45-00A198917708}"/>
+              </c:ext>
+            </c:extLst>
           </c:dPt>
           <c:dPt>
             <c:idx val="11"/>
@@ -859,6 +924,11 @@
               </a:ln>
               <a:effectLst/>
             </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000018-988E-4A34-BC45-00A198917708}"/>
+              </c:ext>
+            </c:extLst>
           </c:dPt>
           <c:dPt>
             <c:idx val="12"/>
@@ -876,6 +946,11 @@
               </a:ln>
               <a:effectLst/>
             </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{0000001A-988E-4A34-BC45-00A198917708}"/>
+              </c:ext>
+            </c:extLst>
           </c:dPt>
           <c:dPt>
             <c:idx val="13"/>
@@ -893,6 +968,11 @@
               </a:ln>
               <a:effectLst/>
             </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{0000001C-988E-4A34-BC45-00A198917708}"/>
+              </c:ext>
+            </c:extLst>
           </c:dPt>
           <c:dPt>
             <c:idx val="14"/>
@@ -907,6 +987,11 @@
               </a:ln>
               <a:effectLst/>
             </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{0000001E-988E-4A34-BC45-00A198917708}"/>
+              </c:ext>
+            </c:extLst>
           </c:dPt>
           <c:cat>
             <c:strRef>
@@ -1009,6 +1094,11 @@
               </c:numCache>
             </c:numRef>
           </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{0000001F-988E-4A34-BC45-00A198917708}"/>
+            </c:ext>
+          </c:extLst>
         </c:ser>
         <c:dLbls>
           <c:showLegendKey val="0"/>
@@ -1189,7 +1279,7 @@
 </file>
 
 <file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
   <c:lang val="ru-RU"/>
   <c:roundedCorners val="0"/>
@@ -1282,6 +1372,11 @@
               </c:numCache>
             </c:numRef>
           </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-C6F9-4BDA-9D15-7134C44EA040}"/>
+            </c:ext>
+          </c:extLst>
         </c:ser>
         <c:ser>
           <c:idx val="1"/>
@@ -1395,6 +1490,11 @@
               </c:numCache>
             </c:numRef>
           </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-C6F9-4BDA-9D15-7134C44EA040}"/>
+            </c:ext>
+          </c:extLst>
         </c:ser>
         <c:dLbls>
           <c:showLegendKey val="0"/>
@@ -1563,7 +1663,7 @@
 </file>
 
 <file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
   <c:lang val="ru-RU"/>
   <c:roundedCorners val="0"/>
@@ -1640,6 +1740,11 @@
               </c:numCache>
             </c:numRef>
           </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-7BF5-4FEB-BF14-FEE5B5C46C5B}"/>
+            </c:ext>
+          </c:extLst>
         </c:ser>
         <c:ser>
           <c:idx val="1"/>
@@ -1697,6 +1802,11 @@
               </c:numCache>
             </c:numRef>
           </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-7BF5-4FEB-BF14-FEE5B5C46C5B}"/>
+            </c:ext>
+          </c:extLst>
         </c:ser>
         <c:dLbls>
           <c:showLegendKey val="0"/>
@@ -1718,7 +1828,7 @@
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="l"/>
-        <c:numFmt formatCode="dd/mm/yy;@" sourceLinked="1"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
@@ -3352,7 +3462,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -3362,8 +3472,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:O41"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A25" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="E45" sqref="E45"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:D3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3375,30 +3485,30 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A1" s="31"/>
-      <c r="B1" s="31"/>
-      <c r="C1" s="31"/>
-      <c r="D1" s="31"/>
+      <c r="A1" s="34"/>
+      <c r="B1" s="34"/>
+      <c r="C1" s="34"/>
+      <c r="D1" s="34"/>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A2" s="29" t="s">
-        <v>30</v>
-      </c>
-      <c r="B2" s="30"/>
-      <c r="C2" s="30"/>
-      <c r="D2" s="30"/>
+      <c r="A2" s="32" t="s">
+        <v>29</v>
+      </c>
+      <c r="B2" s="33"/>
+      <c r="C2" s="33"/>
+      <c r="D2" s="33"/>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A3" s="30"/>
-      <c r="B3" s="30"/>
-      <c r="C3" s="30"/>
-      <c r="D3" s="30"/>
+      <c r="A3" s="33"/>
+      <c r="B3" s="33"/>
+      <c r="C3" s="33"/>
+      <c r="D3" s="33"/>
     </row>
     <row r="4" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A4" s="32"/>
-      <c r="B4" s="33"/>
-      <c r="C4" s="33"/>
-      <c r="D4" s="33"/>
+      <c r="A4" s="35"/>
+      <c r="B4" s="36"/>
+      <c r="C4" s="36"/>
+      <c r="D4" s="36"/>
     </row>
     <row r="5" spans="1:4" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A5" s="8" t="s">
@@ -3634,47 +3744,47 @@
         <v>43551</v>
       </c>
       <c r="G19" s="19"/>
-      <c r="H19" s="36" t="s">
+      <c r="H19" s="30" t="s">
         <v>26</v>
       </c>
-      <c r="I19" s="36"/>
-      <c r="J19" s="36"/>
+      <c r="I19" s="30"/>
+      <c r="J19" s="30"/>
     </row>
     <row r="20" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A20" s="34" t="s">
-        <v>29</v>
-      </c>
-      <c r="B20" s="34"/>
-      <c r="C20" s="34"/>
-      <c r="D20" s="34"/>
-      <c r="G20" s="31"/>
-      <c r="H20" s="31"/>
-      <c r="I20" s="31"/>
-      <c r="J20" s="31"/>
+      <c r="A20" s="37" t="s">
+        <v>28</v>
+      </c>
+      <c r="B20" s="37"/>
+      <c r="C20" s="37"/>
+      <c r="D20" s="37"/>
+      <c r="G20" s="34"/>
+      <c r="H20" s="34"/>
+      <c r="I20" s="34"/>
+      <c r="J20" s="34"/>
     </row>
     <row r="21" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A21" s="35"/>
-      <c r="B21" s="35"/>
-      <c r="C21" s="35"/>
-      <c r="D21" s="35"/>
+      <c r="A21" s="38"/>
+      <c r="B21" s="38"/>
+      <c r="C21" s="38"/>
+      <c r="D21" s="38"/>
       <c r="G21" s="20"/>
-      <c r="H21" s="36" t="s">
-        <v>27</v>
-      </c>
-      <c r="I21" s="36"/>
-      <c r="J21" s="36"/>
+      <c r="H21" s="30" t="s">
+        <v>30</v>
+      </c>
+      <c r="I21" s="30"/>
+      <c r="J21" s="30"/>
     </row>
     <row r="22" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A22" s="35"/>
-      <c r="B22" s="35"/>
-      <c r="C22" s="35"/>
-      <c r="D22" s="35"/>
+      <c r="A22" s="38"/>
+      <c r="B22" s="38"/>
+      <c r="C22" s="38"/>
+      <c r="D22" s="38"/>
     </row>
     <row r="23" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A23" s="35"/>
-      <c r="B23" s="35"/>
-      <c r="C23" s="35"/>
-      <c r="D23" s="35"/>
+      <c r="A23" s="38"/>
+      <c r="B23" s="38"/>
+      <c r="C23" s="38"/>
+      <c r="D23" s="38"/>
     </row>
     <row r="24" spans="1:15" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A24" s="23" t="s">
@@ -3763,18 +3873,18 @@
       <c r="D30" s="22"/>
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A35" s="38" t="s">
-        <v>28</v>
-      </c>
-      <c r="B35" s="36"/>
-      <c r="C35" s="36"/>
-      <c r="D35" s="36"/>
+      <c r="A35" s="29" t="s">
+        <v>27</v>
+      </c>
+      <c r="B35" s="30"/>
+      <c r="C35" s="30"/>
+      <c r="D35" s="30"/>
     </row>
     <row r="36" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A36" s="37"/>
-      <c r="B36" s="37"/>
-      <c r="C36" s="37"/>
-      <c r="D36" s="37"/>
+      <c r="A36" s="31"/>
+      <c r="B36" s="31"/>
+      <c r="C36" s="31"/>
+      <c r="D36" s="31"/>
     </row>
     <row r="37" spans="1:4" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A37" s="23" t="s">
@@ -3816,7 +3926,7 @@
         <v>1</v>
       </c>
       <c r="D39" s="7">
-        <f t="shared" ref="D39:D41" si="3">B39+C39</f>
+        <f t="shared" ref="D39" si="3">B39+C39</f>
         <v>43529</v>
       </c>
     </row>
@@ -3852,14 +3962,14 @@
     </row>
   </sheetData>
   <mergeCells count="8">
+    <mergeCell ref="H19:J19"/>
+    <mergeCell ref="H21:J21"/>
+    <mergeCell ref="G20:J20"/>
     <mergeCell ref="A35:D36"/>
     <mergeCell ref="A2:D3"/>
     <mergeCell ref="A1:D1"/>
     <mergeCell ref="A4:D4"/>
     <mergeCell ref="A20:D23"/>
-    <mergeCell ref="H19:J19"/>
-    <mergeCell ref="H21:J21"/>
-    <mergeCell ref="G20:J20"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>

</xml_diff>